<commit_message>
add sql case expression
</commit_message>
<xml_diff>
--- a/sql_lib.xlsx
+++ b/sql_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
   <si>
     <t>Language</t>
   </si>
@@ -409,6 +409,17 @@
   </si>
   <si>
     <t>Read Active LNP00301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT CUBK, CUNBR, CUSTAT,    
+  case custat                  
+  when 'R' then 'assigned'     
+  when ' ' then 'n/a'          
+  end                          
+FROM zusrlib/cup00301          </t>
+  </si>
+  <si>
+    <t>Case expression</t>
   </si>
 </sst>
 </file>
@@ -818,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="37.5" customHeight="1"/>
@@ -1209,6 +1220,17 @@
       </c>
       <c r="C35" s="4" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="37.5" customHeight="1">
+      <c r="A36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sql entry about cast string/numeric to date format
</commit_message>
<xml_diff>
--- a/sql_lib.xlsx
+++ b/sql_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
   <si>
     <t>Language</t>
   </si>
@@ -426,6 +426,13 @@
   </si>
   <si>
     <t xml:space="preserve">SELECT TRIM(LXMEMO)||'$' FROM ifrs201608/bdplkg0816  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select YEAR(TIMESTAMP_FORMAT(DIGITS(BDPPOSTD),'YYYYMMDD')) 
+ from iprod/bdppay                                          </t>
+  </si>
+  <si>
+    <t>Parse string/numeric to date</t>
   </si>
 </sst>
 </file>
@@ -835,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="37.5" customHeight="1"/>
@@ -1248,6 +1255,17 @@
       </c>
       <c r="C37" s="3" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="37.5" customHeight="1">
+      <c r="A38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sql lib entry about date diff calc in db2
</commit_message>
<xml_diff>
--- a/sql_lib.xlsx
+++ b/sql_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
   <si>
     <t>Language</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>insert into mylhist (CUSTHS,STATHS,PGRPHS,PTYPHS,AMTHS)  select CUSTHS,STATHS,PGRPHS,PTYPHS,AMTHS from mylhist#1</t>
-  </si>
-  <si>
-    <t>SQL</t>
   </si>
   <si>
     <t>SELECT dmacct,dmcmcn,dmcbal, B.DBJACN, B.DBJCCY FROM zusrlib/tap00201 a,ymyles/dbtspf b 
@@ -433,6 +430,19 @@
   </si>
   <si>
     <t>Parse string/numeric to date</t>
+  </si>
+  <si>
+    <t>Date diff</t>
+  </si>
+  <si>
+    <t>DB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select BDPNOTE,                                                                 
+       DAYS(TIMESTAMP_FORMAT(DIGITS(BDPEFFD),'YYYYMMDD')) -
+       DAYS(TIMESTAMP_FORMAT(DIGITS(BDPDUED),'YYYYMMDD'))  
+from ymyles/bdppay                                         
+where bdpeffd - bdpdued &gt;0                                 </t>
   </si>
 </sst>
 </file>
@@ -842,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="37.5" customHeight="1"/>
@@ -861,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -869,32 +879,32 @@
     </row>
     <row r="2" spans="1:4" ht="37.5" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="37.5" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="37.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
@@ -902,370 +912,381 @@
     </row>
     <row r="5" spans="1:4" ht="37.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="37.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="37.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="37.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="37.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="37.5" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="37.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="37.5" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="37.5" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="37.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="37.5" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="37.5" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="37.5" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="37.5" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="37.5" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="37.5" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="37.5" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="37.5" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="37.5" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="37.5" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="37.5" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="37.5" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="37.5" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="37.5" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="37.5" customHeight="1">
       <c r="A29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="37.5" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="37.5" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="37.5" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="37.5" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="37.5" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="37.5" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="37.5" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="37.5" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="37.5" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="37.5" customHeight="1">
+      <c r="A39" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>69</v>
+      <c r="C39" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a sql case recipe about finding key set of a file
</commit_message>
<xml_diff>
--- a/sql_lib.xlsx
+++ b/sql_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
   <si>
     <t>Language</t>
   </si>
@@ -443,6 +443,27 @@
        DAYS(TIMESTAMP_FORMAT(DIGITS(BDPDUED),'YYYYMMDD'))  
 from ymyles/bdppay                                         
 where bdpeffd - bdpdued &gt;0                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receipee: distinguish which file is bigger for 2 version of file with same structure </t>
+  </si>
+  <si>
+    <t>1. Find out the key set of the file structure, if below 2 sqls are both 0, means the set can be used to key this 2 files:
+&gt;    SELECT count(*)                       
+&gt;    FROM zusrlib/lnp00701                 
+&gt;    GROUP BY lhnote, lhrecn, lhpost        
+&gt;    having count(*) &gt; 1;
+&gt;    SELECT count(*)                       
+&gt;    FROM ieom/lnp00701                 
+&gt;    GROUP BY lhnote, lhrecn, lhpost        
+&gt;    having count(*) &gt; 1                   
+2. Use the key set to calculation how much common record between 2 files:
+&gt;    select count(*)                            
+&gt;    from ifrs201110/lnp00701                   
+&gt;    where (lhnote, lhrecn, lhpost) not in (    
+&gt;        select lhnote, lhrecn, lhpost              
+&gt;        from ifrs201111/lnp00701                   
+&gt;    )  ;</t>
   </si>
 </sst>
 </file>
@@ -852,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="37.5" customHeight="1"/>
@@ -1287,6 +1308,17 @@
       </c>
       <c r="C39" s="4" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="37.5" customHeight="1">
+      <c r="A40" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>